<commit_message>
Comiited changes for FB
</commit_message>
<xml_diff>
--- a/src/test/resources/com/testdata/TestData.xlsx
+++ b/src/test/resources/com/testdata/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrca\Downloads\Maven-Failsafe-Plugin-Example-master\src\test\resources\com\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrca\Documents\Automation base framework\Automation Frwk\mavne_failsafe_test\src\test\resources\com\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="0" windowWidth="18090" windowHeight="7830"/>
+    <workbookView xWindow="2595" yWindow="0" windowWidth="18090" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,20 +26,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>vchavarria</t>
+    <t>vicchava@hotmail.com</t>
   </si>
   <si>
-    <t>Maricruzr1979</t>
+    <t>Maricruzr1976</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,13 +70,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -350,17 +361,17 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -368,6 +379,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>